<commit_message>
versión estable de los dos excel
</commit_message>
<xml_diff>
--- a/Excel Dashboard/bin/Debug/3.2.2.2 REGISTRO DE PROGRAMACIÓN DE ENTREGAS.xlsx
+++ b/Excel Dashboard/bin/Debug/3.2.2.2 REGISTRO DE PROGRAMACIÓN DE ENTREGAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\source\repos\Excel Dashboard\Excel Dashboard\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4C8E1A-7D44-4BD5-BDF4-7E12662CAF1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22682E24-2C77-45A1-8B0E-05BA1D2731F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Fecha</t>
   </si>
@@ -100,27 +100,15 @@
     <t>0024</t>
   </si>
   <si>
-    <t>Jorge Gamez</t>
-  </si>
-  <si>
     <t>Por Cobrar</t>
   </si>
   <si>
-    <t>Herrería San Simón</t>
-  </si>
-  <si>
     <t>Contado</t>
   </si>
   <si>
-    <t>Antonio Galindo</t>
-  </si>
-  <si>
     <t>Crédito</t>
   </si>
   <si>
-    <t>Mto Camarillo</t>
-  </si>
-  <si>
     <t>Tipo de entrega</t>
   </si>
   <si>
@@ -145,9 +133,6 @@
     <t>Daniel</t>
   </si>
   <si>
-    <t xml:space="preserve">centro </t>
-  </si>
-  <si>
     <t>San Juan</t>
   </si>
   <si>
@@ -206,6 +191,27 @@
   </si>
   <si>
     <t>Queja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centro </t>
+  </si>
+  <si>
+    <t>Michelle P Simón</t>
+  </si>
+  <si>
+    <t>Lucy Martinez</t>
+  </si>
+  <si>
+    <t>chamacon</t>
+  </si>
+  <si>
+    <t>6 2 1</t>
+  </si>
+  <si>
+    <t>sdsd</t>
+  </si>
+  <si>
+    <t>PUEBLANO</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1372,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,13 +1853,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1912,7 @@
     </row>
     <row r="4" spans="1:29" s="3" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
@@ -1926,19 +1932,19 @@
       <c r="O4" s="58"/>
       <c r="P4" s="59"/>
       <c r="Q4" s="57" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R4" s="58"/>
       <c r="S4" s="58"/>
       <c r="T4" s="59"/>
       <c r="U4" s="57" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="V4" s="58"/>
       <c r="W4" s="58"/>
       <c r="X4" s="59"/>
       <c r="Y4" s="62" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="Z4" s="58"/>
       <c r="AA4" s="58"/>
@@ -1962,7 +1968,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>3</v>
@@ -1995,43 +2001,43 @@
         <v>7</v>
       </c>
       <c r="Q5" s="54" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="R5" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="T5" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="U5" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="V5" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="W5" s="60" t="s">
+      <c r="X5" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z5" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="X5" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z5" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA5" s="63" t="s">
-        <v>53</v>
-      </c>
       <c r="AB5" s="64" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="AC5" s="65" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -2042,14 +2048,14 @@
         <v>20</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G6" s="48">
         <v>1</v>
@@ -2058,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="J6" s="53">
         <v>0.37222222222222223</v>
@@ -2073,13 +2079,13 @@
         <v>0.41319444444444442</v>
       </c>
       <c r="N6" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O6" s="50" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P6" s="52" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="5"/>
@@ -2103,16 +2109,16 @@
         <v>21</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D7" s="34">
         <v>895</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G7" s="45">
         <v>1</v>
@@ -2121,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J7" s="40">
         <v>0.35416666666666669</v>
@@ -2136,13 +2142,13 @@
         <v>0.43402777777777773</v>
       </c>
       <c r="N7" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="P7" s="41" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -2153,14 +2159,14 @@
         <v>22</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="45">
         <v>1</v>
@@ -2169,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J8" s="40">
         <v>0.49305555555555558</v>
@@ -2184,13 +2190,13 @@
         <v>0.53611111111111109</v>
       </c>
       <c r="N8" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O8" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="41" t="s">
         <v>34</v>
-      </c>
-      <c r="P8" s="41" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -2201,16 +2207,16 @@
         <v>23</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D9" s="34">
         <v>876</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G9" s="45">
         <v>2</v>
@@ -2219,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J9" s="40">
         <v>0.66041666666666665</v>
@@ -2234,13 +2240,24 @@
         <v>0.70694444444444438</v>
       </c>
       <c r="N9" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>12121</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versión estable después dos archivos
</commit_message>
<xml_diff>
--- a/Excel Dashboard/bin/Debug/3.2.2.2 REGISTRO DE PROGRAMACIÓN DE ENTREGAS.xlsx
+++ b/Excel Dashboard/bin/Debug/3.2.2.2 REGISTRO DE PROGRAMACIÓN DE ENTREGAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\source\repos\Excel Dashboard\Excel Dashboard\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22682E24-2C77-45A1-8B0E-05BA1D2731F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C35F1A-71CF-4B91-9CC4-C75335E8C9E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Fecha</t>
   </si>
@@ -208,10 +208,7 @@
     <t>6 2 1</t>
   </si>
   <si>
-    <t>sdsd</t>
-  </si>
-  <si>
-    <t>PUEBLANO</t>
+    <t>CALABAZA</t>
   </si>
 </sst>
 </file>
@@ -221,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +283,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +330,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -752,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -943,6 +955,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1853,19 +1868,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="12"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
@@ -2199,65 +2214,81 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+    <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="C9" s="68">
+        <v>43738</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="41"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
         <v>43287</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C10" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D10" s="34">
         <v>876</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F10" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G10" s="45">
         <v>2</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H10" s="33">
         <v>1</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J10" s="40">
         <v>0.66041666666666665</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K10" s="40">
         <v>0.6777777777777777</v>
       </c>
-      <c r="L9" s="40">
+      <c r="L10" s="40">
         <v>0.68888888888888899</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M10" s="40">
         <v>0.70694444444444438</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="46" t="s">
+      <c r="O10" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="P10" s="41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>12121</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2286,7 +2317,7 @@
       <formula>NOT(ISERROR(SEARCH("Urgente",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+  <conditionalFormatting sqref="F8:F9">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Express">
       <formula>NOT(ISERROR(SEARCH("Express",F8)))</formula>
     </cfRule>
@@ -2297,28 +2328,28 @@
       <formula>NOT(ISERROR(SEARCH("Urgente",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
+  <conditionalFormatting sqref="F10">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Express">
-      <formula>NOT(ISERROR(SEARCH("Express",F9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Express",F10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Ordinario">
-      <formula>NOT(ISERROR(SEARCH("Ordinario",F9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Ordinario",F10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Urgente">
-      <formula>NOT(ISERROR(SEARCH("Urgente",F9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Urgente",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Por Cobrar,Contado,Crédito"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Urgente,Ordinario,Express"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O10" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"U01,U02,U03,U04,U05"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H9" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"1,2,3,4"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>